<commit_message>
pyinstaller and bug fixes
</commit_message>
<xml_diff>
--- a/outputs/recommended_class_plan.xlsx
+++ b/outputs/recommended_class_plan.xlsx
@@ -452,19 +452,19 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>CPSC 6179</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CYBR 6126</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>CPSC 6185</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>CPSC 6179</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>CYBR 6126</t>
-        </is>
-      </c>
       <c r="E3" t="inlineStr">
         <is>
           <t>CPSC 6109</t>
@@ -472,22 +472,22 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
+          <t>CPSC 6177</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>CPSC 6175</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>CPSC 6127</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
           <t>CPSC 6119</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>CPSC 6175</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>CPSC 6177</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>CPSC 6127</t>
         </is>
       </c>
     </row>
@@ -563,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Completed courses scheduled again: ['CPSC 6185', 'CPSC 6179', 'CYBR 6126', 'CPSC 6109', 'CPSC 6119', 'CPSC 6175', 'CPSC 6177', 'CPSC 6127']</t>
+          <t>Completed courses scheduled again: ['CPSC 6179', 'CYBR 6126', 'CPSC 6185', 'CPSC 6177', 'CPSC 6175', 'CPSC 6127', 'CPSC 6109', 'CPSC 6119']</t>
         </is>
       </c>
     </row>

</xml_diff>